<commit_message>
plotting .pngs and minor fixes
</commit_message>
<xml_diff>
--- a/kep.xlsx
+++ b/kep.xlsx
@@ -10,13 +10,14 @@
     <sheet name="year" sheetId="1" r:id="rId1"/>
     <sheet name="quarter" sheetId="2" r:id="rId2"/>
     <sheet name="month" sheetId="3" r:id="rId3"/>
+    <sheet name="variables" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="97">
   <si>
     <t>CONSTR_bln_rub_fix</t>
   </si>
@@ -177,7 +178,136 @@
     <t>IND_PROD_ytd</t>
   </si>
   <si>
-    <t>###</t>
+    <t>Код</t>
+  </si>
+  <si>
+    <t>Описание</t>
+  </si>
+  <si>
+    <t>Ед.изм.</t>
+  </si>
+  <si>
+    <t>Объем работ по виду деятельности "Строительство"</t>
+  </si>
+  <si>
+    <t>Кредиторская задолженность</t>
+  </si>
+  <si>
+    <t>алкогольные напитки</t>
+  </si>
+  <si>
+    <t>продукты питания</t>
+  </si>
+  <si>
+    <t>&lt;...&gt;</t>
+  </si>
+  <si>
+    <t>Индекс потребительских цен</t>
+  </si>
+  <si>
+    <t>Индекс промышленного производства</t>
+  </si>
+  <si>
+    <t>Инвестиции в основной капитал</t>
+  </si>
+  <si>
+    <t>Автобусы, штук</t>
+  </si>
+  <si>
+    <t>Автомобили легковые, тыс.штук</t>
+  </si>
+  <si>
+    <t>Грузовые автомобили, тыс.штук</t>
+  </si>
+  <si>
+    <t>Велосипеды (без детских), тыс.штук</t>
+  </si>
+  <si>
+    <t>Электроэнергия, млрд. кВт·ч</t>
+  </si>
+  <si>
+    <t>Вагоны грузовые магистральные, штук</t>
+  </si>
+  <si>
+    <t>Вагоны пассажирские магистральные, штук</t>
+  </si>
+  <si>
+    <t>Оборот розничной торговли</t>
+  </si>
+  <si>
+    <t>Официальный курс евро по отношению к рублю</t>
+  </si>
+  <si>
+    <t>Официальный курс доллара США</t>
+  </si>
+  <si>
+    <t>Численность занятого в экономике населения</t>
+  </si>
+  <si>
+    <t>Средний размер назначенных пенсий</t>
+  </si>
+  <si>
+    <t>Общая численность безработных</t>
+  </si>
+  <si>
+    <t>Уровень безработицы</t>
+  </si>
+  <si>
+    <t>Среднемесячная номинальная начисленная заработная плата одного работника</t>
+  </si>
+  <si>
+    <t>Коммерческий грузооборот транспорта</t>
+  </si>
+  <si>
+    <t>Freight loading on railway transport</t>
+  </si>
+  <si>
+    <t>Грузооборот транспорта, включая коммерческий и некоммерческий грузооборот</t>
+  </si>
+  <si>
+    <t>Объем платных услуг населению</t>
+  </si>
+  <si>
+    <t>млрд. руб. (в фикс. ценах)</t>
+  </si>
+  <si>
+    <t>в % к предыдущему периоду</t>
+  </si>
+  <si>
+    <t>в % к аналог. периоду предыдущего года</t>
+  </si>
+  <si>
+    <t>млрд. руб.</t>
+  </si>
+  <si>
+    <t>штук</t>
+  </si>
+  <si>
+    <t>тыс.</t>
+  </si>
+  <si>
+    <t>млрд. кВт·ч</t>
+  </si>
+  <si>
+    <t>на конец периода</t>
+  </si>
+  <si>
+    <t>млн. человек</t>
+  </si>
+  <si>
+    <t>рублей</t>
+  </si>
+  <si>
+    <t>млрд.</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>млрд. т-км</t>
+  </si>
+  <si>
+    <t>млн. т</t>
   </si>
 </sst>
 </file>
@@ -12153,9 +12283,7 @@
       <c r="AU3" s="2">
         <v>283.3</v>
       </c>
-      <c r="AV3" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="AV3" s="2"/>
       <c r="AW3" s="2"/>
       <c r="AX3" s="2">
         <v>28.7</v>
@@ -43394,4 +43522,714 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>